<commit_message>
import rules from paper; re-order
merge rules from all three sources (writeup.lhs, Rewrites.hs,
paper notes) and re-order the markers in the file.
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
   <si>
     <t xml:space="preserve">streamFilter</t>
   </si>
@@ -95,6 +95,24 @@
   </si>
   <si>
     <t xml:space="preserve">map f . merge s1 s2 = merge (map f s1) (map f s2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">streamFilter f . streamExpand = streamExpand .streamMap (filter f)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">streamWindow . StreamMap f = streamMap (map f) . streamWindow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requires a custom windowmaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reorders?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">streamMerge [streamExpand s1, streamExpand s2,…] = streamExpand . StreamMerge [s1,s2,…]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StreamExpand . StreamMerge [s1,s2,…] = streamMerge [streamExpand s1, streamExpand s2…]</t>
   </si>
   <si>
     <t xml:space="preserve">we would need the inverse of the map predicate</t>
@@ -131,11 +149,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -169,6 +188,13 @@
       <sz val="10"/>
       <name val="Noto Sans"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -233,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,6 +306,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -359,10 +389,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B14:R35"/>
+  <dimension ref="B14:R39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,11 +403,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="3.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="90.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="14" customFormat="false" ht="74.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="2"/>
       <c r="F14" s="3" t="s">
         <v>0</v>
@@ -404,7 +434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
@@ -454,7 +484,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="5"/>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="5" t="n">
         <v>10</v>
       </c>
       <c r="K16" s="6" t="s">
@@ -474,7 +504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="4" t="s">
         <v>2</v>
       </c>
@@ -508,7 +538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="4" t="s">
         <v>3</v>
       </c>
@@ -534,7 +564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="4" t="s">
         <v>4</v>
       </c>
@@ -549,7 +579,9 @@
       <c r="L19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="5"/>
+      <c r="M19" s="5" t="n">
+        <v>11</v>
+      </c>
       <c r="N19" s="8"/>
       <c r="P19" s="9" t="n">
         <v>5</v>
@@ -562,7 +594,9 @@
       <c r="E20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="5" t="n">
+        <v>9</v>
+      </c>
       <c r="G20" s="5" t="n">
         <v>3</v>
       </c>
@@ -575,7 +609,9 @@
       <c r="L20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="5"/>
+      <c r="M20" s="5" t="n">
+        <v>12</v>
+      </c>
       <c r="N20" s="8"/>
       <c r="P20" s="9" t="n">
         <v>6</v>
@@ -584,7 +620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="4" t="s">
         <v>6</v>
       </c>
@@ -619,7 +655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="4" t="s">
         <v>7</v>
       </c>
@@ -636,7 +672,9 @@
         <v>15</v>
       </c>
       <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="K22" s="5" t="n">
+        <v>13</v>
+      </c>
       <c r="L22" s="7" t="s">
         <v>10</v>
       </c>
@@ -654,98 +692,124 @@
       <c r="P23" s="9" t="n">
         <v>9</v>
       </c>
+      <c r="Q23" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P24" s="9" t="n">
         <v>10</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="10"/>
       <c r="C25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
+      <c r="P25" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="Q26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P26" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
-      <c r="F27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P27" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q27" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
-      <c r="F28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>28</v>
-      </c>
+      <c r="Q28" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F33" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="6" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add labelled tabled of pairs to the spreadsheet
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
   <si>
     <t xml:space="preserve">streamFilter</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">streamMerge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">←labelling unique operator pairs</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
@@ -392,10 +395,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B14:R40"/>
+  <dimension ref="B1:R40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -410,6 +413,268 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="74.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="2"/>
       <c r="F14" s="3" t="s">
@@ -442,35 +707,35 @@
         <v>0</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="I15" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M15" s="5" t="n">
         <v>7</v>
       </c>
       <c r="N15" s="8"/>
       <c r="P15" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H16" s="5" t="n">
         <v>5</v>
@@ -491,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L16" s="5" t="n">
         <v>6</v>
@@ -504,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,33 +777,33 @@
         <v>2</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N17" s="8"/>
       <c r="P17" s="9" t="n">
         <v>3</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,13 +814,13 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -564,7 +829,7 @@
         <v>4</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,21 +837,21 @@
         <v>4</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M19" s="5" t="n">
         <v>11</v>
@@ -596,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,7 +875,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -618,7 +883,7 @@
         <v>4</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M20" s="5" t="n">
         <v>12</v>
@@ -628,7 +893,7 @@
         <v>6</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,34 +901,34 @@
         <v>6</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P21" s="9" t="n">
         <v>7</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,28 +942,28 @@
         <v>7</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>13</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P22" s="9" t="n">
         <v>8</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,7 +971,7 @@
         <v>9</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,10 +990,10 @@
         <v>11</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,7 +1004,7 @@
         <v>12</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,7 +1015,7 @@
         <v>13</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,76 +1026,76 @@
     </row>
     <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F33" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F39" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update rewrite rule numbers to match cell number
the numbers in the filled-in table correspond to the cell number in
the index table above. One fewer sets of numbers to worry about.
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -397,8 +397,8 @@
   </sheetPr>
   <dimension ref="B1:R40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -743,30 +743,30 @@
         <v>1</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="M16" s="5" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N16" s="8"/>
       <c r="P16" s="9" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>15</v>
@@ -800,7 +800,7 @@
       </c>
       <c r="N17" s="8"/>
       <c r="P17" s="9" t="n">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>17</v>
@@ -826,7 +826,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="8"/>
       <c r="P18" s="9" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>19</v>
@@ -854,11 +854,11 @@
         <v>11</v>
       </c>
       <c r="M19" s="5" t="n">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="N19" s="8"/>
       <c r="P19" s="9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>21</v>
@@ -869,28 +869,30 @@
         <v>5</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="J20" s="5" t="n">
+        <v>44</v>
+      </c>
       <c r="K20" s="5" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="M20" s="5" t="n">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="N20" s="8"/>
       <c r="P20" s="9" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>22</v>
@@ -925,21 +927,21 @@
         <v>23</v>
       </c>
       <c r="P21" s="9" t="n">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>16</v>
@@ -951,7 +953,7 @@
         <v>11</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>11</v>
@@ -959,8 +961,11 @@
       <c r="M22" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="O22" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="P22" s="9" t="n">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>25</v>
@@ -968,7 +973,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="9" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>26</v>
@@ -976,7 +981,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P24" s="9" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>27</v>
@@ -987,7 +992,7 @@
       <c r="C25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="9" t="n">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="Q25" s="0" t="s">
         <v>28</v>
@@ -1001,7 +1006,7 @@
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="P26" s="9" t="n">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>30</v>
@@ -1012,7 +1017,7 @@
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="P27" s="9" t="n">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="Q27" s="0" t="s">
         <v>31</v>
@@ -1022,6 +1027,9 @@
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
+      <c r="P28" s="9" t="n">
+        <v>44</v>
+      </c>
       <c r="Q28" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
bump cell numbers in spreadsheet
I numbered from 1 in the adoc, so bump the spreadsheet to match
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="B1:R40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,28 +445,28 @@
         <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>8</v>
@@ -477,28 +477,28 @@
         <v>1</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,28 +506,28 @@
         <v>2</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,28 +535,28 @@
         <v>3</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,28 +564,28 @@
         <v>4</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,28 +593,28 @@
         <v>5</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,28 +622,28 @@
         <v>6</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,28 +651,28 @@
         <v>7</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="69.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,7 +728,7 @@
         <v>13</v>
       </c>
       <c r="M15" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N15" s="8"/>
       <c r="P15" s="0" t="s">
@@ -743,30 +743,30 @@
         <v>1</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M16" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N16" s="8"/>
       <c r="P16" s="9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>15</v>
@@ -800,7 +800,7 @@
       </c>
       <c r="N17" s="8"/>
       <c r="P17" s="9" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>17</v>
@@ -854,11 +854,11 @@
         <v>11</v>
       </c>
       <c r="M19" s="5" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N19" s="8"/>
       <c r="P19" s="9" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>21</v>
@@ -869,30 +869,30 @@
         <v>5</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="M20" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N20" s="8"/>
       <c r="P20" s="9" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>22</v>
@@ -927,7 +927,7 @@
         <v>23</v>
       </c>
       <c r="P21" s="9" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>24</v>
@@ -938,10 +938,10 @@
         <v>7</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>16</v>
@@ -953,7 +953,7 @@
         <v>11</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>11</v>
@@ -962,10 +962,10 @@
         <v>9</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P22" s="9" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>25</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="9" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>26</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P24" s="9" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>27</v>
@@ -992,7 +992,7 @@
       <c r="C25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="9" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q25" s="0" t="s">
         <v>28</v>
@@ -1006,7 +1006,7 @@
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="P26" s="9" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>30</v>
@@ -1017,7 +1017,7 @@
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="P27" s="9" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q27" s="0" t="s">
         <v>31</v>
@@ -1028,7 +1028,7 @@
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="P28" s="9" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q28" s="12"/>
     </row>

</xml_diff>

<commit_message>
rational for stream{Map,Scan} . streamFilter{,Acc}
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
   <si>
     <t xml:space="preserve">streamFilter</t>
   </si>
@@ -397,8 +397,8 @@
   </sheetPr>
   <dimension ref="B1:R40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -772,7 +772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="4" t="s">
         <v>2</v>
       </c>
@@ -785,7 +785,9 @@
       <c r="H17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="J17" s="7" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
second example of scanExpand with caveat
Alternative to counter (something a bit like a slope detector but
not quite). The caveat is to do with type unification: it's forced
the stream type to Integer which is not ideal (Ord is needed but
it shouldn't be stricter than that)
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -404,7 +404,7 @@
   <dimension ref="B1:R40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q31" activeCellId="0" sqref="Q31"/>
+      <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1061,76 +1061,76 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="F32" s="0" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="F34" s="0" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="F35" s="0" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="F36" s="0" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="F38" s="0" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="0" t="s">
+      <c r="E40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rule out streamFilter*. streamScan
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
   <si>
     <t xml:space="preserve">streamFilter</t>
   </si>
@@ -76,6 +76,9 @@
     <t xml:space="preserve">map f . expand = expand . Map (map f)</t>
   </si>
   <si>
+    <t xml:space="preserve">x⁷</t>
+  </si>
+  <si>
     <t xml:space="preserve">x⁶</t>
   </si>
   <si>
@@ -142,7 +145,7 @@
     <t xml:space="preserve">I think impossible, I haven’t managed it (nor ruled it out)</t>
   </si>
   <si>
-    <t xml:space="preserve">x⁷</t>
+    <t xml:space="preserve">we can’t compose the filter predicate with somehting that behaves as if w ehad the accumulator without it (consider: counter)</t>
   </si>
   <si>
     <t xml:space="preserve">Accumulator behaviour may be dependent on precisely what events it sees; splitting/joining pre/post would alter that</t>
@@ -403,8 +406,8 @@
   </sheetPr>
   <dimension ref="B1:R40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,15 +819,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="H18" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="I18" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>11</v>
@@ -839,7 +846,7 @@
         <v>45</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,7 +865,7 @@
         <v>11</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L19" s="7" t="s">
         <v>11</v>
@@ -871,7 +878,7 @@
         <v>11</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,7 +914,7 @@
         <v>15</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,34 +922,34 @@
         <v>6</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P21" s="9" t="n">
         <v>58</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,7 +987,7 @@
         <v>57</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,7 +995,7 @@
         <v>41</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,7 +1003,7 @@
         <v>13</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,10 +1014,10 @@
         <v>40</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,7 +1028,7 @@
         <v>48</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,7 +1039,7 @@
         <v>62</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,7 +1056,7 @@
         <v>12</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,7 +1064,7 @@
         <v>44</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,23 +1072,23 @@
         <v>10</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,7 +1096,7 @@
         <v>12</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,20 +1104,23 @@
         <v>13</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="6" t="s">
-        <v>40</v>
+      <c r="F37" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,12 +1128,12 @@
         <v>16</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,7 +1141,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rule out streamMap . streamScan
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t xml:space="preserve">streamFilter</t>
   </si>
@@ -79,6 +79,9 @@
     <t xml:space="preserve">x⁷</t>
   </si>
   <si>
+    <t xml:space="preserve">x⁹</t>
+  </si>
+  <si>
     <t xml:space="preserve">x⁶</t>
   </si>
   <si>
@@ -151,7 +154,7 @@
     <t xml:space="preserve">Accumulator behaviour may be dependent on precisely what events it sees; splitting/joining pre/post would alter that</t>
   </si>
   <si>
-    <t xml:space="preserve">x⁹</t>
+    <t xml:space="preserve">the streamMap output is fed back into scan / can’t be separated</t>
   </si>
   <si>
     <t xml:space="preserve">TODO explain why this is ruled out</t>
@@ -406,8 +409,8 @@
   </sheetPr>
   <dimension ref="B1:R40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -826,12 +829,14 @@
       <c r="F18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="H18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>11</v>
@@ -846,7 +851,7 @@
         <v>45</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,7 +870,7 @@
         <v>11</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L19" s="7" t="s">
         <v>11</v>
@@ -878,7 +883,7 @@
         <v>11</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,7 +919,7 @@
         <v>15</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,34 +927,34 @@
         <v>6</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P21" s="9" t="n">
         <v>58</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,7 +992,7 @@
         <v>57</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,7 +1000,7 @@
         <v>41</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,7 +1008,7 @@
         <v>13</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,10 +1019,10 @@
         <v>40</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,7 +1033,7 @@
         <v>48</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +1044,7 @@
         <v>62</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,7 +1061,7 @@
         <v>12</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,7 +1069,7 @@
         <v>44</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,23 +1077,23 @@
         <v>10</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,7 +1101,7 @@
         <v>12</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,15 +1109,15 @@
         <v>13</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1120,7 +1125,7 @@
         <v>18</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,12 +1133,15 @@
         <v>16</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="6" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add streamJoin . streamScan
</commit_message>
<xml_diff>
--- a/table of operators.xlsx
+++ b/table of operators.xlsx
@@ -409,8 +409,8 @@
   </sheetPr>
   <dimension ref="B1:R40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -844,7 +844,9 @@
       <c r="K18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="5" t="n">
+        <v>31</v>
+      </c>
       <c r="M18" s="5"/>
       <c r="N18" s="8"/>
       <c r="P18" s="9" t="n">

</xml_diff>